<commit_message>
INS script completed - TC02 for Doc OD
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
+++ b/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B88CB6-0F15-4478-9301-BD6ECD4F1549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECB423C-4A69-4614-B212-A63D173F36EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -87,8 +87,8 @@
 coalesce(p.principal_investigators, '') AS `Principal Investigators`,
 coalesce(p.principal_investigators, '') AS `Program Officers`,
 coalesce(p.lead_doc, '')AS `Lead DOC`,
-coalesce(p.lead_doc, '')AS `Activity Code`,
-coalesce(p.award_amount, '') AS `Award Amount`,
+SUBSTRING(p.project_id, 1, 3) AS `Activity code`,
+"$" + apoc.number.format(toInteger(p.award_amount)) AS `Award Amount`,
 coalesce(p.project_end_date, '') AS `Project End Date`,
 coalesce(p.fiscal_year,'')AS `Fiscal Year`</t>
   </si>
@@ -464,7 +464,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
corrected INS profile and qa table obj
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
+++ b/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECB423C-4A69-4614-B212-A63D173F36EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27EF8206-187B-480D-B5C0-26F327E679C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 coalesce (pgm.program_id, '')AS `Program`,
 coalesce(p.project_title, '') AS `Project Title`,
 coalesce(p.principal_investigators, '') AS `Principal Investigators`,
-coalesce(p.principal_investigators, '') AS `Program Officers`,
+coalesce(p.program_officers, '') AS `Program Officers`,
 coalesce(p.lead_doc, '')AS `Lead DOC`,
 SUBSTRING(p.project_id, 1, 3) AS `Activity code`,
 "$" + apoc.number.format(toInteger(p.award_amount)) AS `Award Amount`,
@@ -464,7 +464,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
INS - CCG test case
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
+++ b/InputFiles/TC01_INS_Filter_Doc-CCG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\CDS Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation Latest\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C08376-648D-4A29-BCC7-D90519B0D1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B3BD8E-4659-4E14-AC30-86990DF64B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -53,28 +53,6 @@
   </si>
   <si>
     <t>TC01_INS_Filter_Doc-CCG_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>ProjectsTab</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(pr:project)
- where pr.lead_doc='CCG'
-OPTIONAL MATCH (pr)&lt;--(pub:publication)
-OPTIONAL MATCH (pr)&lt;--(:publication)&lt;--(dt)
-WHERE dt:geo OR dt:sra OR dt:dbgap
-OPTIONAL MATCH (ct:clinical_trial)
-WHERE EXISTS((ct)--&gt;(:publication)--&gt;(pr)) OR EXISTS((pr)&lt;--(ct))
-OPTIONAL MATCH (pr)&lt;--(pat)
-WHERE pat:granted_patent OR pat:patent_application
-WITH p, pr, pub, dt, ct, pat
-RETURN 
-COUNT(DISTINCT p.program_id)  AS Programs,
-COUNT(DISTINCT pr.project_id) as Projects,
-COUNT(DISTINCT pub.publication_id) as Publications,
- COUNT(DISTINCT dt.accession) as Datasets,
-  COUNT(DISTINCT ct.clinical_trial_id) as `Clinical Trials`,
-COUNT(DISTINCT pat.patent_id) as Patents</t>
   </si>
   <si>
     <t>DatasetsTab</t>
@@ -185,6 +163,29 @@
     COALESCE(dt.release_date,'') AS `Release Date`,
     COALESCE(dt.registration_date,'') AS `Registration Date`
     order by Accession ASC</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(pr:project)
+where pr.lead_doc='CCG'
+OPTIONAL MATCH (pr)&lt;--(pub:publication)
+OPTIONAL MATCH (ct:clinical_trial)
+WHERE EXISTS((pr)&lt;--(pub)&lt;--(ct)) OR EXISTS((pr)&lt;--(ct))
+OPTIONAL MATCH (pr)&lt;--(pat)
+WHERE pat:patent_application OR pat:granted_patent
+OPTIONAL MATCH (pr)&lt;-[*1..2]-(dt)
+WHERE dt:sra OR dt:dbgap OR dt:geo
+WITH p, pr, pub, ct, pat, dt
+RETURN
+COUNT(DISTINCT p.program_id) AS Programs,
+COUNT(DISTINCT pr.queried_project_id) AS Projects,
+COUNT(DISTINCT pr.project_id) AS Grants,
+COUNT(DISTINCT pub.publication_id) AS Publications,
+COUNT(DISTINCT dt.accession) AS Datasets,
+COUNT(DISTINCT ct.clinical_trial_id) AS `Clinical Trials`,
+COUNT(DISTINCT pat.patent_id) AS Patents</t>
+  </si>
+  <si>
+    <t>GrantsTab</t>
   </si>
 </sst>
 </file>
@@ -557,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,15 +588,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -606,13 +607,13 @@
     </row>
     <row r="3" spans="1:5" ht="390" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -623,13 +624,13 @@
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -640,13 +641,13 @@
     </row>
     <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -657,13 +658,13 @@
     </row>
     <row r="6" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>

</xml_diff>